<commit_message>
upd - computed mass flux estimates via linear regression.
</commit_message>
<xml_diff>
--- a/doc_load_estimates.xlsx
+++ b/doc_load_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D25DD03-8320-DF41-8F87-467D2A35506B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A42AAFD-4657-4B4C-B2CD-3CCA6473B4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="660" windowWidth="35840" windowHeight="17440" xr2:uid="{F8E1E424-3AB0-7F47-9B3D-F48A33B90D72}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{F8E1E424-3AB0-7F47-9B3D-F48A33B90D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,10 +217,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,9 +258,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,6 +265,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -586,7 +590,8 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -640,25 +645,31 @@
       <c r="C2" s="2">
         <v>1346</v>
       </c>
-      <c r="D2" s="6" cm="1">
+      <c r="D2" s="5" cm="1">
         <f t="array" ref="D2:D16">(C2:C16 * 1000) / 141</f>
         <v>9546.099290780141</v>
       </c>
       <c r="E2" s="2">
         <v>338</v>
       </c>
-      <c r="F2" s="6" cm="1">
+      <c r="F2" s="5" cm="1">
         <f t="array" ref="F2:F16">(E2:E16 * 1000) / 141</f>
         <v>2397.1631205673757</v>
       </c>
       <c r="G2" s="2">
         <v>900</v>
       </c>
-      <c r="H2" s="6" cm="1">
+      <c r="H2" s="5" cm="1">
         <f t="array" ref="H2:H16">(G2:G16 * 1000) / 141</f>
         <v>6382.9787234042551</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="8">
+        <v>1909</v>
+      </c>
+      <c r="J2" s="9" cm="1">
+        <f t="array" ref="J2:J16">(I2:I16 * 1000) / 141</f>
+        <v>13539.007092198581</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
@@ -670,22 +681,27 @@
       <c r="C3" s="2">
         <v>2520</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>17872.340425531915</v>
       </c>
       <c r="E3" s="2">
         <v>1284</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>9106.3829787234044</v>
       </c>
       <c r="G3" s="2">
         <v>2023</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>14347.517730496455</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="8">
+        <v>2705</v>
+      </c>
+      <c r="J3" s="9">
+        <v>19184.397163120568</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
@@ -697,22 +713,27 @@
       <c r="C4" s="2">
         <v>1363</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>9666.6666666666661</v>
       </c>
       <c r="E4" s="2">
         <v>683</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>4843.9716312056735</v>
       </c>
       <c r="G4" s="2">
         <v>885</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>6276.5957446808507</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="8">
+        <v>814</v>
+      </c>
+      <c r="J4" s="9">
+        <v>5773.0496453900705</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
@@ -724,22 +745,27 @@
       <c r="C5" s="2">
         <v>8030</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>56950.354609929076</v>
       </c>
       <c r="E5" s="2">
         <v>2921</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>20716.312056737588</v>
       </c>
       <c r="G5" s="2">
         <v>6326</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>44865.248226950353</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="8">
+        <v>8022</v>
+      </c>
+      <c r="J5" s="9">
+        <v>56893.617021276594</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
@@ -751,22 +777,27 @@
       <c r="C6" s="2">
         <v>650</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>4609.9290780141846</v>
       </c>
       <c r="E6" s="2">
         <v>140</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>992.9078014184397</v>
       </c>
       <c r="G6" s="2">
         <v>427</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>3028.3687943262412</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="8">
+        <v>502</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3560.2836879432625</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
@@ -778,22 +809,27 @@
       <c r="C7" s="2">
         <v>950</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>6737.5886524822699</v>
       </c>
       <c r="E7" s="2">
         <v>770</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>5460.9929078014184</v>
       </c>
       <c r="G7" s="2">
         <v>871</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>6177.3049645390074</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="8">
+        <v>852</v>
+      </c>
+      <c r="J7" s="9">
+        <v>6042.5531914893618</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
@@ -805,22 +841,27 @@
       <c r="C8" s="2">
         <v>8913</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>63212.765957446805</v>
       </c>
       <c r="E8" s="2">
         <v>4176</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>29617.021276595744</v>
       </c>
       <c r="G8" s="3">
         <v>7287</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>51680.851063829788</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="8">
+        <v>9022</v>
+      </c>
+      <c r="J8" s="9">
+        <v>63985.815602836883</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
@@ -832,22 +873,27 @@
       <c r="C9" s="2">
         <v>4382</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>31078.014184397161</v>
       </c>
       <c r="E9" s="4">
         <v>1138</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>8070.921985815603</v>
       </c>
       <c r="G9" s="2">
         <v>3453</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>24489.361702127659</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="8">
+        <v>5180</v>
+      </c>
+      <c r="J9" s="9">
+        <v>36737.588652482271</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
@@ -859,22 +905,27 @@
       <c r="C10" s="2">
         <v>3417</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>24234.042553191488</v>
       </c>
       <c r="E10" s="4">
         <v>3165</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>22446.808510638297</v>
       </c>
       <c r="G10" s="2">
         <v>3291</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>23340.425531914894</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="8">
+        <v>3274</v>
+      </c>
+      <c r="J10" s="9">
+        <v>23219.858156028367</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
@@ -886,22 +937,27 @@
       <c r="C11" s="2">
         <v>861</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>6106.3829787234044</v>
       </c>
       <c r="E11" s="2">
         <v>655</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>4645.3900709219861</v>
       </c>
       <c r="G11" s="2">
         <v>758</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>5375.8865248226948</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="8">
+        <v>752</v>
+      </c>
+      <c r="J11" s="9">
+        <v>5333.333333333333</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
@@ -913,22 +969,27 @@
       <c r="C12" s="2">
         <v>1924</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>13645.390070921985</v>
       </c>
       <c r="E12" s="2">
         <v>1287</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>9127.6595744680853</v>
       </c>
       <c r="G12" s="2">
         <v>1732</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>12283.687943262412</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="8">
+        <v>2364</v>
+      </c>
+      <c r="J12" s="9">
+        <v>16765.957446808512</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
@@ -940,22 +1001,27 @@
       <c r="C13" s="2">
         <v>1587</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>11255.319148936171</v>
       </c>
       <c r="E13" s="2">
         <v>961</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>6815.6028368794323</v>
       </c>
       <c r="G13" s="2">
         <v>1375</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>9751.7730496453896</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="8">
+        <v>1453</v>
+      </c>
+      <c r="J13" s="9">
+        <v>10304.964539007093</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
@@ -967,22 +1033,27 @@
       <c r="C14" s="2">
         <v>5960</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>42269.503546099288</v>
       </c>
       <c r="E14" s="2">
         <v>3543</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>25127.659574468085</v>
       </c>
       <c r="G14" s="2">
         <v>5161</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>36602.836879432623</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="8">
+        <v>5660</v>
+      </c>
+      <c r="J14" s="9">
+        <v>40141.843971631206</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
@@ -994,22 +1065,27 @@
       <c r="C15" s="2">
         <v>1165</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>8262.411347517731</v>
       </c>
       <c r="E15" s="2">
         <v>693</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>4914.8936170212764</v>
       </c>
       <c r="G15" s="2">
         <v>982</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>6964.5390070921985</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="8">
+        <v>1021</v>
+      </c>
+      <c r="J15" s="9">
+        <v>7241.1347517730501</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
@@ -1021,22 +1097,27 @@
       <c r="C16" s="2">
         <v>845</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>5992.9078014184397</v>
       </c>
       <c r="E16" s="2">
         <v>611</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>4333.333333333333</v>
       </c>
       <c r="G16" s="2">
         <v>791</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>5609.9290780141846</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="8">
+        <v>940</v>
+      </c>
+      <c r="J16" s="9">
+        <v>6666.666666666667</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week of June 5th-9th work
</commit_message>
<xml_diff>
--- a/doc_load_estimates.xlsx
+++ b/doc_load_estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/MSc/R/thesis_data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1DE260-DE2C-4342-9AAD-2DFB5FFD3A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D55A8CD-D10C-914E-94D0-80F880EAB1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="33440" windowHeight="21100" xr2:uid="{F8E1E424-3AB0-7F47-9B3D-F48A33B90D72}"/>
+    <workbookView xWindow="11740" yWindow="500" windowWidth="17060" windowHeight="17500" xr2:uid="{F8E1E424-3AB0-7F47-9B3D-F48A33B90D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>site</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>linear interpolation (g C/m^2/season)</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Harvest</t>
+  </si>
+  <si>
+    <t>Insect</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -584,538 +599,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A574C0AA-01B3-2B46-BE68-4A1F72AE1574}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A14" activeCellId="2" sqref="A11:XFD11 A12:XFD12 A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="35.1640625" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" customWidth="1"/>
-    <col min="10" max="10" width="33.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" customWidth="1"/>
+    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>9542.7000000000007</v>
       </c>
-      <c r="D2" s="4" cm="1">
-        <f t="array" ref="D2:D16">(C2:C16 / 1000)</f>
+      <c r="E2" s="4" cm="1">
+        <f t="array" ref="E2:E16">(D2:D16 / 1000)</f>
         <v>9.5427</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2397.4</v>
       </c>
-      <c r="F2" s="4" cm="1">
-        <f t="array" ref="F2:F16">(E2:E16 / 1000)</f>
+      <c r="G2" s="4" cm="1">
+        <f t="array" ref="G2:G16">(F2:F16 / 1000)</f>
         <v>2.3974000000000002</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>6386</v>
       </c>
-      <c r="H2" s="8" cm="1">
-        <f t="array" ref="H2:H16">(G2:G16 / 1000)</f>
+      <c r="I2" s="8" cm="1">
+        <f t="array" ref="I2:I16">(H2:H16 / 1000)</f>
         <v>6.3860000000000001</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>13539.8</v>
       </c>
-      <c r="J2" s="8" cm="1">
-        <f t="array" ref="J2:J16">(I2:I16 / 1000)</f>
+      <c r="K2" s="8" cm="1">
+        <f t="array" ref="K2:K16">(J2:J16 / 1000)</f>
         <v>13.5398</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>17870.3</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>17.8703</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>9109.2999999999993</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>9.1092999999999993</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>14349</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>14.349</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>19184.5</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="8">
         <v>19.1845</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>9665.5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>9.6654999999999998</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>4841.1000000000004</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>4.8411</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>6278.8</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>6.2788000000000004</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>5769.8</v>
       </c>
-      <c r="J4" s="8">
+      <c r="K4" s="8">
         <v>5.7698</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>56952.9</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>56.9529</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>20719.099999999999</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>20.719099999999997</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>44868.1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>44.868099999999998</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>56892.4</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>56.892400000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>4560.8</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>4.5608000000000004</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>984.7</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>0.98470000000000002</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>3027.2</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>3.0271999999999997</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="8">
         <v>3561</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>3.5609999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>6721.5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>6.7214999999999998</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>5449.1</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>5.4491000000000005</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>6181.8</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>6.1818</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>6045.5</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>6.0454999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>63212.9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>63.212900000000005</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>29616.799999999999</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>29.616799999999998</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>51682.3</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>51.682300000000005</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>63987.5</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>63.987499999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>31077.4</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>31.077400000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>8068.7</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>8.0686999999999998</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>24486.9</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="8">
         <v>24.486900000000002</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>36734.6</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>36.7346</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>24231.5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>24.2315</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>22445.4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>22.445400000000003</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>23339.599999999999</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <v>23.339599999999997</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J10" s="8">
         <v>23220.400000000001</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>23.220400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="4">
         <v>6107.2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>6.1071999999999997</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>4644.5</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>4.6444999999999999</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>5376.8</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <v>5.3768000000000002</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>5331.3</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>5.3313000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>13986.2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>13.9862</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>9359.4</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>9.3593999999999991</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>12281.2</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>12.2812</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <v>16765.400000000001</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>16.765400000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>11225.8</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>11.2258</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>6795.1</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>6.7951000000000006</v>
       </c>
-      <c r="G13" s="5">
+      <c r="H13" s="5">
         <v>9755</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>9.7550000000000008</v>
       </c>
-      <c r="I13" s="6">
+      <c r="J13" s="6">
         <v>10306.799999999999</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>10.306799999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>41798.1</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>41.798099999999998</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>24847.4</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>24.8474</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>36605.199999999997</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>36.605199999999996</v>
       </c>
-      <c r="I14" s="8">
+      <c r="J14" s="8">
         <v>40139.9</v>
       </c>
-      <c r="J14" s="8">
+      <c r="K14" s="8">
         <v>40.139900000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>8242.5</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>8.2424999999999997</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>4904.5</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>4.9044999999999996</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="6">
         <v>6964.2</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>6.9641999999999999</v>
       </c>
-      <c r="I15" s="7">
+      <c r="J15" s="7">
         <v>7239.1</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>7.2391000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="4">
         <v>5990.8</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>5.9908000000000001</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>4334.8999999999996</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>4.3348999999999993</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>5608.4</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <v>5.6083999999999996</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="7">
         <v>6665.4</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K16" s="8">
         <v>6.6654</v>
       </c>
     </row>

</xml_diff>